<commit_message>
adloori to davuluri completed
</commit_message>
<xml_diff>
--- a/Adloori_LabExam03Grading.xlsx
+++ b/Adloori_LabExam03Grading.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S533574\Desktop\44542 Spring 2019\Lab Exams\Lab Exam 03\LabExam3Rubrics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LabExam3Rubrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -405,6 +405,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -415,18 +427,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1505,8 +1505,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1520,14 +1520,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
@@ -1562,7 +1562,9 @@
       <c r="D3" s="5">
         <v>1</v>
       </c>
-      <c r="E3" s="5"/>
+      <c r="E3" s="5">
+        <v>1</v>
+      </c>
       <c r="F3" s="13"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1576,7 +1578,9 @@
       <c r="D4" s="2">
         <v>2</v>
       </c>
-      <c r="E4" s="2"/>
+      <c r="E4" s="2">
+        <v>2</v>
+      </c>
       <c r="F4" s="13"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1590,7 +1594,9 @@
       <c r="D5" s="2">
         <v>2</v>
       </c>
-      <c r="E5" s="2"/>
+      <c r="E5" s="2">
+        <v>2</v>
+      </c>
       <c r="F5" s="13"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1604,34 +1610,36 @@
       <c r="D6" s="18">
         <v>2</v>
       </c>
-      <c r="E6" s="18"/>
+      <c r="E6" s="18">
+        <v>2</v>
+      </c>
       <c r="F6" s="19"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="29" t="s">
+      <c r="A7" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="30"/>
-      <c r="C7" s="31"/>
+      <c r="B7" s="27"/>
+      <c r="C7" s="28"/>
       <c r="D7" s="6">
         <f>SUM(D3:D6)</f>
         <v>7</v>
       </c>
       <c r="E7" s="6">
         <f>SUM(E3:E6)</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F7" s="6"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="25" t="s">
+      <c r="A8" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="25"/>
-      <c r="C8" s="25"/>
-      <c r="D8" s="25"/>
-      <c r="E8" s="25"/>
-      <c r="F8" s="25"/>
+      <c r="B8" s="29"/>
+      <c r="C8" s="29"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="29"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
@@ -1664,7 +1672,9 @@
       <c r="D10" s="2">
         <v>2</v>
       </c>
-      <c r="E10" s="2"/>
+      <c r="E10" s="2">
+        <v>2</v>
+      </c>
       <c r="F10" s="13"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -1678,7 +1688,9 @@
       <c r="D11" s="2">
         <v>2</v>
       </c>
-      <c r="E11" s="2"/>
+      <c r="E11" s="2">
+        <v>2</v>
+      </c>
       <c r="F11" s="13"/>
     </row>
     <row r="12" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1692,7 +1704,9 @@
       <c r="D12" s="2">
         <v>2</v>
       </c>
-      <c r="E12" s="2"/>
+      <c r="E12" s="2">
+        <v>2</v>
+      </c>
       <c r="F12" s="13"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -1706,7 +1720,9 @@
       <c r="D13" s="2">
         <v>2</v>
       </c>
-      <c r="E13" s="2"/>
+      <c r="E13" s="2">
+        <v>2</v>
+      </c>
       <c r="F13" s="13"/>
     </row>
     <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1722,34 +1738,36 @@
       <c r="D14" s="18">
         <v>2</v>
       </c>
-      <c r="E14" s="18"/>
+      <c r="E14" s="18">
+        <v>2</v>
+      </c>
       <c r="F14" s="19"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="29" t="s">
+      <c r="A15" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="B15" s="30"/>
-      <c r="C15" s="31"/>
+      <c r="B15" s="27"/>
+      <c r="C15" s="28"/>
       <c r="D15" s="6">
         <f>SUM(D10:D14)</f>
         <v>10</v>
       </c>
       <c r="E15" s="6">
         <f>SUM(E10:E14)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F15" s="6"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="25" t="s">
+      <c r="A16" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="25"/>
-      <c r="C16" s="25"/>
-      <c r="D16" s="25"/>
-      <c r="E16" s="25"/>
-      <c r="F16" s="25"/>
+      <c r="B16" s="29"/>
+      <c r="C16" s="29"/>
+      <c r="D16" s="29"/>
+      <c r="E16" s="29"/>
+      <c r="F16" s="29"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
@@ -1904,11 +1922,11 @@
       <c r="F25" s="19"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="29" t="s">
+      <c r="A26" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="B26" s="30"/>
-      <c r="C26" s="31"/>
+      <c r="B26" s="27"/>
+      <c r="C26" s="28"/>
       <c r="D26" s="6">
         <f>SUM(D18:D25)</f>
         <v>56</v>
@@ -1920,14 +1938,14 @@
       <c r="F26" s="6"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="25" t="s">
+      <c r="A27" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="B27" s="25"/>
-      <c r="C27" s="25"/>
-      <c r="D27" s="25"/>
-      <c r="E27" s="25"/>
-      <c r="F27" s="25"/>
+      <c r="B27" s="29"/>
+      <c r="C27" s="29"/>
+      <c r="D27" s="29"/>
+      <c r="E27" s="29"/>
+      <c r="F27" s="29"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="14" t="s">
@@ -1988,11 +2006,11 @@
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="29" t="s">
+      <c r="A31" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="B31" s="30"/>
-      <c r="C31" s="31"/>
+      <c r="B31" s="27"/>
+      <c r="C31" s="28"/>
       <c r="D31" s="6">
         <f>SUM(D29:D30)</f>
         <v>20</v>
@@ -2004,14 +2022,14 @@
       <c r="F31" s="6"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="25" t="s">
+      <c r="A32" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="B32" s="25"/>
-      <c r="C32" s="25"/>
-      <c r="D32" s="25"/>
-      <c r="E32" s="25"/>
-      <c r="F32" s="25"/>
+      <c r="B32" s="29"/>
+      <c r="C32" s="29"/>
+      <c r="D32" s="29"/>
+      <c r="E32" s="29"/>
+      <c r="F32" s="29"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="14" t="s">
@@ -2054,11 +2072,11 @@
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="29" t="s">
+      <c r="A35" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="B35" s="30"/>
-      <c r="C35" s="31"/>
+      <c r="B35" s="27"/>
+      <c r="C35" s="28"/>
       <c r="D35" s="6">
         <f>SUM(D34:D34)</f>
         <v>7</v>
@@ -2070,14 +2088,14 @@
       <c r="F35" s="6"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="26" t="s">
+      <c r="A36" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="B36" s="27"/>
-      <c r="C36" s="27"/>
-      <c r="D36" s="27"/>
-      <c r="E36" s="27"/>
-      <c r="F36" s="28"/>
+      <c r="B36" s="31"/>
+      <c r="C36" s="31"/>
+      <c r="D36" s="31"/>
+      <c r="E36" s="31"/>
+      <c r="F36" s="32"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="7">
@@ -2098,28 +2116,23 @@
       <c r="F37" s="3"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="32" t="s">
+      <c r="A38" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="B38" s="32"/>
-      <c r="C38" s="32"/>
+      <c r="B38" s="25"/>
+      <c r="C38" s="25"/>
       <c r="D38" s="10">
         <f>SUM(D7, D15, D26, D35, D31)</f>
         <v>100</v>
       </c>
       <c r="E38" s="11">
         <f>SUM(E7, E15, E26, E35, E37, E31)</f>
-        <v>41</v>
+        <v>58</v>
       </c>
       <c r="F38" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A38:C38"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="A26:C26"/>
-    <mergeCell ref="A35:C35"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A8:F8"/>
     <mergeCell ref="A16:F16"/>
@@ -2127,6 +2140,11 @@
     <mergeCell ref="A36:F36"/>
     <mergeCell ref="A32:F32"/>
     <mergeCell ref="A31:C31"/>
+    <mergeCell ref="A38:C38"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="A35:C35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>